<commit_message>
Project ready to be deployed.
</commit_message>
<xml_diff>
--- a/structure.xlsx
+++ b/structure.xlsx
@@ -1,16 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sota/Dropbox/2 Business/1 Datons/2 Areas/Courses/03 ML/materials/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846DA4B9-B205-9140-B036-5951F5D184D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Landing"/>
-    <sheet r:id="rId2" sheetId="2" name="Instructions"/>
+    <sheet name="Landing" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -188,8 +207,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -232,87 +250,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C11" displayName="Table2" name="Table2" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:C11"/>
-  <tableColumns count="3">
-    <tableColumn name="ID" id="1"/>
-    <tableColumn name="Type" id="2"/>
-    <tableColumn name="Instruction" id="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A2:E19" totalsRowCount="1">
+  <autoFilter ref="A2:E18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Chapter" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Lesson"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Folder" totalsRowFunction="count"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Provided" totalsRowFunction="count"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Raw" totalsRowFunction="count"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A2:E19" displayName="Table3" name="Table3" id="2" totalsRowCount="1">
-  <autoFilter ref="A2:E18"/>
-  <tableColumns count="5">
-    <tableColumn name="Chapter" id="1" totalsRowLabel="Total"/>
-    <tableColumn name="Lesson" id="2"/>
-    <tableColumn name="Folder" id="3" totalsRowFunction="count"/>
-    <tableColumn name="Provided" id="4" totalsRowFunction="count"/>
-    <tableColumn name="Raw" id="5" totalsRowFunction="count"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Instruction"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -321,10 +333,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -362,71 +374,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,7 +466,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -477,11 +489,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -490,13 +502,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -506,7 +518,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -515,7 +527,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -524,7 +536,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -532,10 +544,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -600,41 +612,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="12" width="28.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="28.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="10" t="s">
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -646,251 +656,208 @@
       <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="10" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="10" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="10" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="10" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="10" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="10" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="10" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="11">
-        <f>subtotal(103,[Folder])</f>
+      <c r="C19" s="9">
+        <f>SUBTOTAL(103,Table3[Folder])</f>
+        <v>12</v>
       </c>
       <c r="D19" s="1">
-        <f>subtotal(103,[Provided])</f>
+        <f>SUBTOTAL(103,Table3[Provided])</f>
+        <v>3</v>
       </c>
       <c r="E19" s="1">
-        <f>subtotal(103,[Raw])</f>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+        <f>SUBTOTAL(103,Table3[Raw])</f>
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -904,7 +871,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -912,14 +879,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="4" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="54.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -941,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -952,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -963,7 +930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -974,7 +941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -985,7 +952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -996,7 +963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1007,7 +974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1018,7 +985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1029,7 +996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>

</xml_diff>